<commit_message>
Auto-committed on 2022/06/06 週一 15:26:10.48
</commit_message>
<xml_diff>
--- a/Program/Other/L4320_LNW171E底稿(10909調息檔)機動-地區別調整.xlsx
+++ b/Program/Other/L4320_LNW171E底稿(10909調息檔)機動-地區別調整.xlsx
@@ -99,15 +99,15 @@
     <t>下次調整日</t>
   </si>
   <si>
-    <t>調整後利率</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>加碼值</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>檢核訊息</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>擬調利率</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1154,10 +1154,10 @@
         <v>9</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q1" s="7" t="s">
         <v>15</v>
@@ -1175,7 +1175,7 @@
         <v>18</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2022/10/12 週三 11:46:06.22
</commit_message>
<xml_diff>
--- a/Program/Other/L4320_LNW171E底稿(10909調息檔)機動-地區別調整.xlsx
+++ b/Program/Other/L4320_LNW171E底稿(10909調息檔)機動-地區別調整.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\itxWrite\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8688"/>
   </bookViews>
   <sheets>
     <sheet name="正常件" sheetId="2" r:id="rId1"/>
@@ -99,15 +99,15 @@
     <t>下次調整日</t>
   </si>
   <si>
-    <t>加碼值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>檢核訊息</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>擬調利率</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>合約加碼值</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1100,7 +1100,7 @@
     <col min="12" max="12" width="10.109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="25.44140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="9.6640625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="9" style="1"/>
+    <col min="15" max="15" width="10.88671875" style="1" customWidth="1"/>
     <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
     <col min="17" max="17" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.21875" style="1" bestFit="1" customWidth="1"/>
@@ -1154,10 +1154,10 @@
         <v>9</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="7" t="s">
         <v>15</v>
@@ -1175,7 +1175,7 @@
         <v>18</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>